<commit_message>
mostrar consumo funcional, faltando mudar casas decimais
</commit_message>
<xml_diff>
--- a/registro.xlsx
+++ b/registro.xlsx
@@ -1043,7 +1043,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="A1:B5"/>
@@ -1066,60 +1066,108 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021-05</t>
+          <t>2021-01</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>521</t>
+          <t>233</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2022-02</t>
+          <t>2021-05</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>222</t>
+          <t>521</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2023-01</t>
+          <t>2022-01</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>123</t>
+          <t>789</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2023-02</t>
+          <t>2022-02</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>223</t>
+          <t>222</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>2023-01</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>123123123</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2023-02</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>223</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
           <t>2023-09</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B8" t="inlineStr">
         <is>
           <t>923</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2023-10</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>550</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2023-11</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>500</t>
         </is>
       </c>
     </row>

</xml_diff>